<commit_message>
update:upload claim, history after save
</commit_message>
<xml_diff>
--- a/public/template/claim.xlsx
+++ b/public/template/claim.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609024DC-7056-DC4B-885C-A0A8246AFE45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D935E2-380C-0744-A31C-0C3AE632C784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5060" yWindow="8100" windowWidth="33600" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>or</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Nomor Polis</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Reas</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
   </si>
 </sst>
 </file>
@@ -378,8 +378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -393,28 +393,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>